<commit_message>
add few more terms
</commit_message>
<xml_diff>
--- a/doc/ontoDog_input/ontoDog_input.xlsx
+++ b/doc/ontoDog_input/ontoDog_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="101">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -301,6 +301,24 @@
   </si>
   <si>
     <t>solid support function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/GO_0008150 </t>
+  </si>
+  <si>
+    <t>biological_process</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000416</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001619</t>
+  </si>
+  <si>
+    <t>specimen collection time measurement datum</t>
+  </si>
+  <si>
+    <t>time measurement datum</t>
   </si>
 </sst>
 </file>
@@ -632,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1148,6 +1166,39 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>